<commit_message>
Fix typo in AQI scale
</commit_message>
<xml_diff>
--- a/assets/aqi-calcs.xlsx
+++ b/assets/aqi-calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmm\Documents\Arduino\sketches\catena4630-test1\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmm\Documents\Arduino\libraries\MCCI-Catena-PMS7003\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AE81B7-FF1D-4EA5-A39C-4E90E81AE8D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6904AB36-12D5-4BC9-83ED-D179E9F2EE16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28065" yWindow="735" windowWidth="23445" windowHeight="12615" xr2:uid="{F9FF6CA9-42F7-4FBF-B779-76C0C00D3E4F}"/>
+    <workbookView xWindow="1185" yWindow="930" windowWidth="15390" windowHeight="9645" xr2:uid="{F9FF6CA9-42F7-4FBF-B779-76C0C00D3E4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill>
@@ -433,149 +433,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF7E0023"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99004C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00E400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99004C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00E400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00E400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7E00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00E400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00E400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00E400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -901,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B3491-3F44-4420-BEF0-1E3912855AC9}">
   <dimension ref="B3:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -980,14 +837,14 @@
         <v>221</v>
       </c>
       <c r="P4">
-        <f>ROUND(VLOOKUP(O4,$F$30:$K$36,5)+(O4-VLOOKUP(O4,$F$30:$K$36,1))/(VLOOKUP(O4,$F$30:$K$36,2)-VLOOKUP(O4,$F$30:$K$36,1))*(VLOOKUP(O4,$F$30:$K$36,6)),0)</f>
+        <f t="shared" ref="P4:P28" si="0">ROUND(VLOOKUP(O4,$F$30:$K$36,5)+(O4-VLOOKUP(O4,$F$30:$K$36,1))/(VLOOKUP(O4,$F$30:$K$36,2)-VLOOKUP(O4,$F$30:$K$36,1))*(VLOOKUP(O4,$F$30:$K$36,6)),0)</f>
         <v>272</v>
       </c>
       <c r="Q4">
         <v>289</v>
       </c>
       <c r="R4">
-        <f>ROUND(VLOOKUP(Q4,$H$30:$K$36,3)+(Q4-VLOOKUP(Q4,$H$30:$K$36,1))/(VLOOKUP(Q4,$H$30:$K$36,2)-VLOOKUP(Q4,$H$30:$K$36,1))*(VLOOKUP(Q4,$H$30:$K$36,4)),0)</f>
+        <f t="shared" ref="R4:R28" si="1">ROUND(VLOOKUP(Q4,$H$30:$K$36,3)+(Q4-VLOOKUP(Q4,$H$30:$K$36,1))/(VLOOKUP(Q4,$H$30:$K$36,2)-VLOOKUP(Q4,$H$30:$K$36,1))*(VLOOKUP(Q4,$H$30:$K$36,4)),0)</f>
         <v>168</v>
       </c>
       <c r="S4" t="s">
@@ -1074,14 +931,14 @@
         <v>394</v>
       </c>
       <c r="P5">
-        <f>ROUND(VLOOKUP(O5,$F$30:$K$36,5)+(O5-VLOOKUP(O5,$F$30:$K$36,1))/(VLOOKUP(O5,$F$30:$K$36,2)-VLOOKUP(O5,$F$30:$K$36,1))*(VLOOKUP(O5,$F$30:$K$36,6)),0)</f>
-        <v>429</v>
+        <f t="shared" si="0"/>
+        <v>430</v>
       </c>
       <c r="Q5">
         <v>501</v>
       </c>
       <c r="R5">
-        <f>ROUND(VLOOKUP(Q5,$H$30:$K$36,3)+(Q5-VLOOKUP(Q5,$H$30:$K$36,1))/(VLOOKUP(Q5,$H$30:$K$36,2)-VLOOKUP(Q5,$H$30:$K$36,1))*(VLOOKUP(Q5,$H$30:$K$36,4)),0)</f>
+        <f t="shared" si="1"/>
         <v>397</v>
       </c>
       <c r="S5" t="s">
@@ -1168,15 +1025,15 @@
         <v>511</v>
       </c>
       <c r="P6">
-        <f>ROUND(VLOOKUP(O6,$F$30:$K$36,5)+(O6-VLOOKUP(O6,$F$30:$K$36,1))/(VLOOKUP(O6,$F$30:$K$36,2)-VLOOKUP(O6,$F$30:$K$36,1))*(VLOOKUP(O6,$F$30:$K$36,6)),0)</f>
-        <v>507</v>
+        <f t="shared" si="0"/>
+        <v>508</v>
       </c>
       <c r="Q6">
         <v>630</v>
       </c>
       <c r="R6">
-        <f>ROUND(VLOOKUP(Q6,$H$30:$K$36,3)+(Q6-VLOOKUP(Q6,$H$30:$K$36,1))/(VLOOKUP(Q6,$H$30:$K$36,2)-VLOOKUP(Q6,$H$30:$K$36,1))*(VLOOKUP(Q6,$H$30:$K$36,4)),0)</f>
-        <v>526</v>
+        <f t="shared" si="1"/>
+        <v>527</v>
       </c>
       <c r="S6" t="s">
         <v>3</v>
@@ -1262,15 +1119,15 @@
         <v>703</v>
       </c>
       <c r="P7">
-        <f>ROUND(VLOOKUP(O7,$F$30:$K$36,5)+(O7-VLOOKUP(O7,$F$30:$K$36,1))/(VLOOKUP(O7,$F$30:$K$36,2)-VLOOKUP(O7,$F$30:$K$36,1))*(VLOOKUP(O7,$F$30:$K$36,6)),0)</f>
-        <v>635</v>
+        <f t="shared" si="0"/>
+        <v>636</v>
       </c>
       <c r="Q7">
         <v>1212</v>
       </c>
       <c r="R7">
-        <f>ROUND(VLOOKUP(Q7,$H$30:$K$36,3)+(Q7-VLOOKUP(Q7,$H$30:$K$36,1))/(VLOOKUP(Q7,$H$30:$K$36,2)-VLOOKUP(Q7,$H$30:$K$36,1))*(VLOOKUP(Q7,$H$30:$K$36,4)),0)</f>
-        <v>1114</v>
+        <f t="shared" si="1"/>
+        <v>1115</v>
       </c>
       <c r="S7" t="s">
         <v>3</v>
@@ -1356,15 +1213,15 @@
         <v>872</v>
       </c>
       <c r="P8">
-        <f>ROUND(VLOOKUP(O8,$F$30:$K$36,5)+(O8-VLOOKUP(O8,$F$30:$K$36,1))/(VLOOKUP(O8,$F$30:$K$36,2)-VLOOKUP(O8,$F$30:$K$36,1))*(VLOOKUP(O8,$F$30:$K$36,6)),0)</f>
-        <v>748</v>
+        <f t="shared" si="0"/>
+        <v>749</v>
       </c>
       <c r="Q8">
         <v>1407</v>
       </c>
       <c r="R8">
-        <f>ROUND(VLOOKUP(Q8,$H$30:$K$36,3)+(Q8-VLOOKUP(Q8,$H$30:$K$36,1))/(VLOOKUP(Q8,$H$30:$K$36,2)-VLOOKUP(Q8,$H$30:$K$36,1))*(VLOOKUP(Q8,$H$30:$K$36,4)),0)</f>
-        <v>1311</v>
+        <f t="shared" si="1"/>
+        <v>1312</v>
       </c>
       <c r="S8" t="s">
         <v>3</v>
@@ -1450,15 +1307,15 @@
         <v>1117</v>
       </c>
       <c r="P9">
-        <f>ROUND(VLOOKUP(O9,$F$30:$K$36,5)+(O9-VLOOKUP(O9,$F$30:$K$36,1))/(VLOOKUP(O9,$F$30:$K$36,2)-VLOOKUP(O9,$F$30:$K$36,1))*(VLOOKUP(O9,$F$30:$K$36,6)),0)</f>
-        <v>911</v>
+        <f t="shared" si="0"/>
+        <v>912</v>
       </c>
       <c r="Q9">
         <v>1769</v>
       </c>
       <c r="R9">
-        <f>ROUND(VLOOKUP(Q9,$H$30:$K$36,3)+(Q9-VLOOKUP(Q9,$H$30:$K$36,1))/(VLOOKUP(Q9,$H$30:$K$36,2)-VLOOKUP(Q9,$H$30:$K$36,1))*(VLOOKUP(Q9,$H$30:$K$36,4)),0)</f>
-        <v>1677</v>
+        <f t="shared" si="1"/>
+        <v>1678</v>
       </c>
       <c r="S9" t="s">
         <v>3</v>
@@ -1544,15 +1401,15 @@
         <v>1329</v>
       </c>
       <c r="P10">
-        <f>ROUND(VLOOKUP(O10,$F$30:$K$36,5)+(O10-VLOOKUP(O10,$F$30:$K$36,1))/(VLOOKUP(O10,$F$30:$K$36,2)-VLOOKUP(O10,$F$30:$K$36,1))*(VLOOKUP(O10,$F$30:$K$36,6)),0)</f>
-        <v>1053</v>
+        <f t="shared" si="0"/>
+        <v>1054</v>
       </c>
       <c r="Q10">
         <v>2275</v>
       </c>
       <c r="R10">
-        <f>ROUND(VLOOKUP(Q10,$H$30:$K$36,3)+(Q10-VLOOKUP(Q10,$H$30:$K$36,1))/(VLOOKUP(Q10,$H$30:$K$36,2)-VLOOKUP(Q10,$H$30:$K$36,1))*(VLOOKUP(Q10,$H$30:$K$36,4)),0)</f>
-        <v>2188</v>
+        <f t="shared" si="1"/>
+        <v>2189</v>
       </c>
       <c r="S10" t="s">
         <v>3</v>
@@ -1638,15 +1495,15 @@
         <v>1524</v>
       </c>
       <c r="P11">
-        <f>ROUND(VLOOKUP(O11,$F$30:$K$36,5)+(O11-VLOOKUP(O11,$F$30:$K$36,1))/(VLOOKUP(O11,$F$30:$K$36,2)-VLOOKUP(O11,$F$30:$K$36,1))*(VLOOKUP(O11,$F$30:$K$36,6)),0)</f>
-        <v>1183</v>
+        <f t="shared" si="0"/>
+        <v>1184</v>
       </c>
       <c r="Q11">
         <v>2853</v>
       </c>
       <c r="R11">
-        <f>ROUND(VLOOKUP(Q11,$H$30:$K$36,3)+(Q11-VLOOKUP(Q11,$H$30:$K$36,1))/(VLOOKUP(Q11,$H$30:$K$36,2)-VLOOKUP(Q11,$H$30:$K$36,1))*(VLOOKUP(Q11,$H$30:$K$36,4)),0)</f>
-        <v>2772</v>
+        <f t="shared" si="1"/>
+        <v>2773</v>
       </c>
       <c r="S11" t="s">
         <v>3</v>
@@ -1732,15 +1589,15 @@
         <v>1707</v>
       </c>
       <c r="P12">
-        <f>ROUND(VLOOKUP(O12,$F$30:$K$36,5)+(O12-VLOOKUP(O12,$F$30:$K$36,1))/(VLOOKUP(O12,$F$30:$K$36,2)-VLOOKUP(O12,$F$30:$K$36,1))*(VLOOKUP(O12,$F$30:$K$36,6)),0)</f>
-        <v>1305</v>
+        <f t="shared" si="0"/>
+        <v>1306</v>
       </c>
       <c r="Q12">
         <v>3327</v>
       </c>
       <c r="R12">
-        <f>ROUND(VLOOKUP(Q12,$H$30:$K$36,3)+(Q12-VLOOKUP(Q12,$H$30:$K$36,1))/(VLOOKUP(Q12,$H$30:$K$36,2)-VLOOKUP(Q12,$H$30:$K$36,1))*(VLOOKUP(Q12,$H$30:$K$36,4)),0)</f>
-        <v>3251</v>
+        <f t="shared" si="1"/>
+        <v>3252</v>
       </c>
       <c r="S12" t="s">
         <v>3</v>
@@ -1826,15 +1683,15 @@
         <v>1919</v>
       </c>
       <c r="P13">
-        <f>ROUND(VLOOKUP(O13,$F$30:$K$36,5)+(O13-VLOOKUP(O13,$F$30:$K$36,1))/(VLOOKUP(O13,$F$30:$K$36,2)-VLOOKUP(O13,$F$30:$K$36,1))*(VLOOKUP(O13,$F$30:$K$36,6)),0)</f>
-        <v>1446</v>
+        <f t="shared" si="0"/>
+        <v>1447</v>
       </c>
       <c r="Q13">
         <v>3776</v>
       </c>
       <c r="R13">
-        <f>ROUND(VLOOKUP(Q13,$H$30:$K$36,3)+(Q13-VLOOKUP(Q13,$H$30:$K$36,1))/(VLOOKUP(Q13,$H$30:$K$36,2)-VLOOKUP(Q13,$H$30:$K$36,1))*(VLOOKUP(Q13,$H$30:$K$36,4)),0)</f>
-        <v>3704</v>
+        <f t="shared" si="1"/>
+        <v>3705</v>
       </c>
       <c r="S13" t="s">
         <v>3</v>
@@ -1920,15 +1777,15 @@
         <v>1808</v>
       </c>
       <c r="P14">
-        <f>ROUND(VLOOKUP(O14,$F$30:$K$36,5)+(O14-VLOOKUP(O14,$F$30:$K$36,1))/(VLOOKUP(O14,$F$30:$K$36,2)-VLOOKUP(O14,$F$30:$K$36,1))*(VLOOKUP(O14,$F$30:$K$36,6)),0)</f>
-        <v>1372</v>
+        <f t="shared" si="0"/>
+        <v>1373</v>
       </c>
       <c r="Q14">
         <v>3616</v>
       </c>
       <c r="R14">
-        <f>ROUND(VLOOKUP(Q14,$H$30:$K$36,3)+(Q14-VLOOKUP(Q14,$H$30:$K$36,1))/(VLOOKUP(Q14,$H$30:$K$36,2)-VLOOKUP(Q14,$H$30:$K$36,1))*(VLOOKUP(Q14,$H$30:$K$36,4)),0)</f>
-        <v>3542</v>
+        <f t="shared" si="1"/>
+        <v>3543</v>
       </c>
       <c r="S14" t="s">
         <v>3</v>
@@ -2014,15 +1871,15 @@
         <v>1675</v>
       </c>
       <c r="P15">
-        <f>ROUND(VLOOKUP(O15,$F$30:$K$36,5)+(O15-VLOOKUP(O15,$F$30:$K$36,1))/(VLOOKUP(O15,$F$30:$K$36,2)-VLOOKUP(O15,$F$30:$K$36,1))*(VLOOKUP(O15,$F$30:$K$36,6)),0)</f>
-        <v>1284</v>
+        <f t="shared" si="0"/>
+        <v>1285</v>
       </c>
       <c r="Q15">
         <v>3448</v>
       </c>
       <c r="R15">
-        <f>ROUND(VLOOKUP(Q15,$H$30:$K$36,3)+(Q15-VLOOKUP(Q15,$H$30:$K$36,1))/(VLOOKUP(Q15,$H$30:$K$36,2)-VLOOKUP(Q15,$H$30:$K$36,1))*(VLOOKUP(Q15,$H$30:$K$36,4)),0)</f>
-        <v>3373</v>
+        <f t="shared" si="1"/>
+        <v>3374</v>
       </c>
       <c r="S15" t="s">
         <v>3</v>
@@ -2108,15 +1965,15 @@
         <v>1578</v>
       </c>
       <c r="P16">
-        <f>ROUND(VLOOKUP(O16,$F$30:$K$36,5)+(O16-VLOOKUP(O16,$F$30:$K$36,1))/(VLOOKUP(O16,$F$30:$K$36,2)-VLOOKUP(O16,$F$30:$K$36,1))*(VLOOKUP(O16,$F$30:$K$36,6)),0)</f>
-        <v>1219</v>
+        <f t="shared" si="0"/>
+        <v>1220</v>
       </c>
       <c r="Q16">
         <v>3342</v>
       </c>
       <c r="R16">
-        <f>ROUND(VLOOKUP(Q16,$H$30:$K$36,3)+(Q16-VLOOKUP(Q16,$H$30:$K$36,1))/(VLOOKUP(Q16,$H$30:$K$36,2)-VLOOKUP(Q16,$H$30:$K$36,1))*(VLOOKUP(Q16,$H$30:$K$36,4)),0)</f>
-        <v>3266</v>
+        <f t="shared" si="1"/>
+        <v>3267</v>
       </c>
       <c r="S16" t="s">
         <v>3</v>
@@ -2202,15 +2059,15 @@
         <v>1395</v>
       </c>
       <c r="P17">
-        <f>ROUND(VLOOKUP(O17,$F$30:$K$36,5)+(O17-VLOOKUP(O17,$F$30:$K$36,1))/(VLOOKUP(O17,$F$30:$K$36,2)-VLOOKUP(O17,$F$30:$K$36,1))*(VLOOKUP(O17,$F$30:$K$36,6)),0)</f>
-        <v>1097</v>
+        <f t="shared" si="0"/>
+        <v>1098</v>
       </c>
       <c r="Q17">
         <v>2771</v>
       </c>
       <c r="R17">
-        <f>ROUND(VLOOKUP(Q17,$H$30:$K$36,3)+(Q17-VLOOKUP(Q17,$H$30:$K$36,1))/(VLOOKUP(Q17,$H$30:$K$36,2)-VLOOKUP(Q17,$H$30:$K$36,1))*(VLOOKUP(Q17,$H$30:$K$36,4)),0)</f>
-        <v>2689</v>
+        <f t="shared" si="1"/>
+        <v>2690</v>
       </c>
       <c r="S17" t="s">
         <v>3</v>
@@ -2296,15 +2153,15 @@
         <v>1233</v>
       </c>
       <c r="P18">
-        <f>ROUND(VLOOKUP(O18,$F$30:$K$36,5)+(O18-VLOOKUP(O18,$F$30:$K$36,1))/(VLOOKUP(O18,$F$30:$K$36,2)-VLOOKUP(O18,$F$30:$K$36,1))*(VLOOKUP(O18,$F$30:$K$36,6)),0)</f>
-        <v>989</v>
+        <f t="shared" si="0"/>
+        <v>990</v>
       </c>
       <c r="Q18">
         <v>2582</v>
       </c>
       <c r="R18">
-        <f>ROUND(VLOOKUP(Q18,$H$30:$K$36,3)+(Q18-VLOOKUP(Q18,$H$30:$K$36,1))/(VLOOKUP(Q18,$H$30:$K$36,2)-VLOOKUP(Q18,$H$30:$K$36,1))*(VLOOKUP(Q18,$H$30:$K$36,4)),0)</f>
-        <v>2498</v>
+        <f t="shared" si="1"/>
+        <v>2499</v>
       </c>
       <c r="S18" t="s">
         <v>3</v>
@@ -2390,15 +2247,15 @@
         <v>991</v>
       </c>
       <c r="P19">
-        <f>ROUND(VLOOKUP(O19,$F$30:$K$36,5)+(O19-VLOOKUP(O19,$F$30:$K$36,1))/(VLOOKUP(O19,$F$30:$K$36,2)-VLOOKUP(O19,$F$30:$K$36,1))*(VLOOKUP(O19,$F$30:$K$36,6)),0)</f>
-        <v>827</v>
+        <f t="shared" si="0"/>
+        <v>828</v>
       </c>
       <c r="Q19">
         <v>2226</v>
       </c>
       <c r="R19">
-        <f>ROUND(VLOOKUP(Q19,$H$30:$K$36,3)+(Q19-VLOOKUP(Q19,$H$30:$K$36,1))/(VLOOKUP(Q19,$H$30:$K$36,2)-VLOOKUP(Q19,$H$30:$K$36,1))*(VLOOKUP(Q19,$H$30:$K$36,4)),0)</f>
-        <v>2138</v>
+        <f t="shared" si="1"/>
+        <v>2139</v>
       </c>
       <c r="S19" t="s">
         <v>3</v>
@@ -2484,15 +2341,15 @@
         <v>803</v>
       </c>
       <c r="P20">
-        <f>ROUND(VLOOKUP(O20,$F$30:$K$36,5)+(O20-VLOOKUP(O20,$F$30:$K$36,1))/(VLOOKUP(O20,$F$30:$K$36,2)-VLOOKUP(O20,$F$30:$K$36,1))*(VLOOKUP(O20,$F$30:$K$36,6)),0)</f>
-        <v>702</v>
+        <f t="shared" si="0"/>
+        <v>703</v>
       </c>
       <c r="Q20">
         <v>1768</v>
       </c>
       <c r="R20">
-        <f>ROUND(VLOOKUP(Q20,$H$30:$K$36,3)+(Q20-VLOOKUP(Q20,$H$30:$K$36,1))/(VLOOKUP(Q20,$H$30:$K$36,2)-VLOOKUP(Q20,$H$30:$K$36,1))*(VLOOKUP(Q20,$H$30:$K$36,4)),0)</f>
-        <v>1676</v>
+        <f t="shared" si="1"/>
+        <v>1677</v>
       </c>
       <c r="S20" t="s">
         <v>3</v>
@@ -2579,14 +2436,14 @@
       </c>
       <c r="P21">
         <f>ROUND(VLOOKUP(O21,$F$30:$K$36,5)+(O21-VLOOKUP(O21,$F$30:$K$36,1))/(VLOOKUP(O21,$F$30:$K$36,2)-VLOOKUP(O21,$F$30:$K$36,1))*(VLOOKUP(O21,$F$30:$K$36,6)),0)</f>
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="Q21">
         <v>1768</v>
       </c>
       <c r="R21">
-        <f>ROUND(VLOOKUP(Q21,$H$30:$K$36,3)+(Q21-VLOOKUP(Q21,$H$30:$K$36,1))/(VLOOKUP(Q21,$H$30:$K$36,2)-VLOOKUP(Q21,$H$30:$K$36,1))*(VLOOKUP(Q21,$H$30:$K$36,4)),0)</f>
-        <v>1676</v>
+        <f t="shared" si="1"/>
+        <v>1677</v>
       </c>
       <c r="S21" t="s">
         <v>3</v>
@@ -2672,15 +2529,15 @@
         <v>607</v>
       </c>
       <c r="P22">
-        <f>ROUND(VLOOKUP(O22,$F$30:$K$36,5)+(O22-VLOOKUP(O22,$F$30:$K$36,1))/(VLOOKUP(O22,$F$30:$K$36,2)-VLOOKUP(O22,$F$30:$K$36,1))*(VLOOKUP(O22,$F$30:$K$36,6)),0)</f>
-        <v>571</v>
+        <f t="shared" si="0"/>
+        <v>572</v>
       </c>
       <c r="Q22">
         <v>1180</v>
       </c>
       <c r="R22">
-        <f>ROUND(VLOOKUP(Q22,$H$30:$K$36,3)+(Q22-VLOOKUP(Q22,$H$30:$K$36,1))/(VLOOKUP(Q22,$H$30:$K$36,2)-VLOOKUP(Q22,$H$30:$K$36,1))*(VLOOKUP(Q22,$H$30:$K$36,4)),0)</f>
-        <v>1082</v>
+        <f t="shared" si="1"/>
+        <v>1083</v>
       </c>
       <c r="S22" t="s">
         <v>3</v>
@@ -2766,15 +2623,15 @@
         <v>402</v>
       </c>
       <c r="P23">
-        <f>ROUND(VLOOKUP(O23,$F$30:$K$36,5)+(O23-VLOOKUP(O23,$F$30:$K$36,1))/(VLOOKUP(O23,$F$30:$K$36,2)-VLOOKUP(O23,$F$30:$K$36,1))*(VLOOKUP(O23,$F$30:$K$36,6)),0)</f>
-        <v>434</v>
+        <f t="shared" si="0"/>
+        <v>435</v>
       </c>
       <c r="Q23">
         <v>663</v>
       </c>
       <c r="R23">
-        <f>ROUND(VLOOKUP(Q23,$H$30:$K$36,3)+(Q23-VLOOKUP(Q23,$H$30:$K$36,1))/(VLOOKUP(Q23,$H$30:$K$36,2)-VLOOKUP(Q23,$H$30:$K$36,1))*(VLOOKUP(Q23,$H$30:$K$36,4)),0)</f>
-        <v>560</v>
+        <f t="shared" si="1"/>
+        <v>561</v>
       </c>
       <c r="S23" t="s">
         <v>3</v>
@@ -2860,14 +2717,14 @@
         <v>191</v>
       </c>
       <c r="P24">
-        <f>ROUND(VLOOKUP(O24,$F$30:$K$36,5)+(O24-VLOOKUP(O24,$F$30:$K$36,1))/(VLOOKUP(O24,$F$30:$K$36,2)-VLOOKUP(O24,$F$30:$K$36,1))*(VLOOKUP(O24,$F$30:$K$36,6)),0)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="Q24">
         <v>213</v>
       </c>
       <c r="R24">
-        <f>ROUND(VLOOKUP(Q24,$H$30:$K$36,3)+(Q24-VLOOKUP(Q24,$H$30:$K$36,1))/(VLOOKUP(Q24,$H$30:$K$36,2)-VLOOKUP(Q24,$H$30:$K$36,1))*(VLOOKUP(Q24,$H$30:$K$36,4)),0)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="S24" t="s">
@@ -2954,14 +2811,14 @@
         <v>85</v>
       </c>
       <c r="P25">
-        <f>ROUND(VLOOKUP(O25,$F$30:$K$36,5)+(O25-VLOOKUP(O25,$F$30:$K$36,1))/(VLOOKUP(O25,$F$30:$K$36,2)-VLOOKUP(O25,$F$30:$K$36,1))*(VLOOKUP(O25,$F$30:$K$36,6)),0)</f>
+        <f t="shared" si="0"/>
         <v>162</v>
       </c>
       <c r="Q25">
         <v>91</v>
       </c>
       <c r="R25">
-        <f>ROUND(VLOOKUP(Q25,$H$30:$K$36,3)+(Q25-VLOOKUP(Q25,$H$30:$K$36,1))/(VLOOKUP(Q25,$H$30:$K$36,2)-VLOOKUP(Q25,$H$30:$K$36,1))*(VLOOKUP(Q25,$H$30:$K$36,4)),0)</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="S25" t="s">
@@ -3009,14 +2866,14 @@
         <v>7</v>
       </c>
       <c r="P26">
-        <f>ROUND(VLOOKUP(O26,$F$30:$K$36,5)+(O26-VLOOKUP(O26,$F$30:$K$36,1))/(VLOOKUP(O26,$F$30:$K$36,2)-VLOOKUP(O26,$F$30:$K$36,1))*(VLOOKUP(O26,$F$30:$K$36,6)),0)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="Q26">
         <v>8</v>
       </c>
       <c r="R26">
-        <f>ROUND(VLOOKUP(Q26,$H$30:$K$36,3)+(Q26-VLOOKUP(Q26,$H$30:$K$36,1))/(VLOOKUP(Q26,$H$30:$K$36,2)-VLOOKUP(Q26,$H$30:$K$36,1))*(VLOOKUP(Q26,$H$30:$K$36,4)),0)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -3025,11 +2882,11 @@
         <v>10</v>
       </c>
       <c r="P27">
-        <f>ROUND(VLOOKUP(O27,$F$30:$K$36,5)+(O27-VLOOKUP(O27,$F$30:$K$36,1))/(VLOOKUP(O27,$F$30:$K$36,2)-VLOOKUP(O27,$F$30:$K$36,1))*(VLOOKUP(O27,$F$30:$K$36,6)),0)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="R27">
-        <f>ROUND(VLOOKUP(Q27,$H$30:$K$36,3)+(Q27-VLOOKUP(Q27,$H$30:$K$36,1))/(VLOOKUP(Q27,$H$30:$K$36,2)-VLOOKUP(Q27,$H$30:$K$36,1))*(VLOOKUP(Q27,$H$30:$K$36,4)),0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T27">
@@ -3065,14 +2922,14 @@
         <v>3</v>
       </c>
       <c r="P28">
-        <f>ROUND(VLOOKUP(O28,$F$30:$K$36,5)+(O28-VLOOKUP(O28,$F$30:$K$36,1))/(VLOOKUP(O28,$F$30:$K$36,2)-VLOOKUP(O28,$F$30:$K$36,1))*(VLOOKUP(O28,$F$30:$K$36,6)),0)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="Q28">
         <v>2</v>
       </c>
       <c r="R28">
-        <f>ROUND(VLOOKUP(Q28,$H$30:$K$36,3)+(Q28-VLOOKUP(Q28,$H$30:$K$36,1))/(VLOOKUP(Q28,$H$30:$K$36,2)-VLOOKUP(Q28,$H$30:$K$36,1))*(VLOOKUP(Q28,$H$30:$K$36,4)),0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -3221,7 +3078,7 @@
         <v>604</v>
       </c>
       <c r="J36">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="K36">
         <v>100</v>

</xml_diff>

<commit_message>
Fix #2: update AQI calculation per 2012 amendment.
</commit_message>
<xml_diff>
--- a/assets/aqi-calcs.xlsx
+++ b/assets/aqi-calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmm\Documents\Arduino\libraries\MCCI-Catena-PMS7003\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6904AB36-12D5-4BC9-83ED-D179E9F2EE16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE74C7D9-113B-4AF2-82DA-502478FCF6E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="930" windowWidth="15390" windowHeight="9645" xr2:uid="{F9FF6CA9-42F7-4FBF-B779-76C0C00D3E4F}"/>
+    <workbookView xWindow="15" yWindow="368" windowWidth="20505" windowHeight="12352" xr2:uid="{F9FF6CA9-42F7-4FBF-B779-76C0C00D3E4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B3491-3F44-4420-BEF0-1E3912855AC9}">
   <dimension ref="B3:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="Q25">
         <v>91</v>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="P26">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="Q26">
         <v>8</v>
@@ -2883,7 +2883,7 @@
       </c>
       <c r="P27">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="R27">
         <f t="shared" si="1"/>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="P28">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Q28">
         <v>2</v>
@@ -2949,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>15.4</v>
+        <v>12</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2966,10 +2966,10 @@
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.45">
       <c r="F31">
-        <v>15.5</v>
+        <v>12.1</v>
       </c>
       <c r="G31">
-        <v>40.4</v>
+        <v>35.4</v>
       </c>
       <c r="H31">
         <v>55</v>
@@ -2986,10 +2986,10 @@
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.45">
       <c r="F32">
-        <v>40.5</v>
+        <v>35.5</v>
       </c>
       <c r="G32">
-        <v>65.400000000000006</v>
+        <v>55.4</v>
       </c>
       <c r="H32">
         <v>155</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="33" spans="6:11" x14ac:dyDescent="0.45">
       <c r="F33">
-        <v>65.5</v>
+        <v>55.5</v>
       </c>
       <c r="G33">
         <v>150.4</v>

</xml_diff>